<commit_message>
`poetry update` and `make all`
</commit_message>
<xml_diff>
--- a/sssom_schema/project/excel/sssom_schema.xlsx
+++ b/sssom_schema/project/excel/sssom_schema.xlsx
@@ -4,11 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -630,6 +632,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mapping_registry_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_set_references</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -763,4 +811,55 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mapping_set_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mirror_from</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>registry_confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mapping_set_group</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>last_updated</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>local_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit for packaging (#194)
* readme in wrong file

* made all folders, packages

* `poetry update` and `make all`
</commit_message>
<xml_diff>
--- a/sssom_schema/project/excel/sssom_schema.xlsx
+++ b/sssom_schema/project/excel/sssom_schema.xlsx
@@ -4,11 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -630,6 +632,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mapping_registry_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_set_references</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -763,4 +811,55 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mapping_set_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mirror_from</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>registry_confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mapping_set_group</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>last_updated</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>local_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>